<commit_message>
Add home page, navigation and theme
</commit_message>
<xml_diff>
--- a/Phd_neuroscience/test.xlsx
+++ b/Phd_neuroscience/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Paolo/Dropbox/Dottorato_neurosciences/2020_2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988FF54D-7222-C44B-8E49-21F5FA8FDCD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D942A23-17F6-5247-A86F-50C13E58689C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5790,8 +5790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E22FF0-3EAE-F842-AB96-E4D6ECC533B0}">
   <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9035,7 +9035,7 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B102">
         <v>45</v>
@@ -9067,7 +9067,7 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B103">
         <v>22</v>
@@ -9099,7 +9099,7 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B104">
         <v>21</v>
@@ -9131,7 +9131,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B105">
         <v>23</v>
@@ -9163,7 +9163,7 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B106">
         <v>21</v>
@@ -9195,7 +9195,7 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B107">
         <v>20</v>
@@ -9227,7 +9227,7 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B108">
         <v>21</v>
@@ -9259,7 +9259,7 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B109">
         <v>19</v>
@@ -9291,7 +9291,7 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B110">
         <v>19</v>
@@ -9323,7 +9323,7 @@
     </row>
     <row r="111" spans="1:10">
       <c r="A111">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B111">
         <v>21</v>
@@ -9355,7 +9355,7 @@
     </row>
     <row r="112" spans="1:10">
       <c r="A112">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B112">
         <v>19</v>
@@ -9387,7 +9387,7 @@
     </row>
     <row r="113" spans="1:10">
       <c r="A113">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B113">
         <v>19</v>
@@ -9419,7 +9419,7 @@
     </row>
     <row r="114" spans="1:10">
       <c r="A114">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B114">
         <v>20</v>
@@ -9451,7 +9451,7 @@
     </row>
     <row r="115" spans="1:10">
       <c r="A115">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B115">
         <v>22</v>
@@ -9483,7 +9483,7 @@
     </row>
     <row r="116" spans="1:10">
       <c r="A116">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B116">
         <v>20</v>
@@ -9515,7 +9515,7 @@
     </row>
     <row r="117" spans="1:10">
       <c r="A117">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B117">
         <v>22</v>
@@ -9547,7 +9547,7 @@
     </row>
     <row r="118" spans="1:10">
       <c r="A118">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B118">
         <v>22</v>
@@ -9579,7 +9579,7 @@
     </row>
     <row r="119" spans="1:10">
       <c r="A119">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B119">
         <v>23</v>
@@ -9611,7 +9611,7 @@
     </row>
     <row r="120" spans="1:10">
       <c r="A120">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="B120">
         <v>23</v>
@@ -9643,7 +9643,7 @@
     </row>
     <row r="121" spans="1:10">
       <c r="A121">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B121">
         <v>26</v>
@@ -9675,7 +9675,7 @@
     </row>
     <row r="122" spans="1:10">
       <c r="A122">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B122">
         <v>33</v>
@@ -9707,7 +9707,7 @@
     </row>
     <row r="123" spans="1:10">
       <c r="A123">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="B123">
         <v>24</v>
@@ -9739,7 +9739,7 @@
     </row>
     <row r="124" spans="1:10">
       <c r="A124">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="B124">
         <v>23</v>
@@ -9771,7 +9771,7 @@
     </row>
     <row r="125" spans="1:10">
       <c r="A125">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B125">
         <v>25</v>
@@ -9803,7 +9803,7 @@
     </row>
     <row r="126" spans="1:10">
       <c r="A126">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="B126">
         <v>22</v>
@@ -9835,7 +9835,7 @@
     </row>
     <row r="127" spans="1:10">
       <c r="A127">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="B127">
         <v>33</v>
@@ -9867,7 +9867,7 @@
     </row>
     <row r="128" spans="1:10">
       <c r="A128">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B128">
         <v>23</v>
@@ -9899,7 +9899,7 @@
     </row>
     <row r="129" spans="1:10">
       <c r="A129">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="B129">
         <v>28</v>
@@ -9931,7 +9931,7 @@
     </row>
     <row r="130" spans="1:10">
       <c r="A130">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="B130">
         <v>25</v>
@@ -9963,7 +9963,7 @@
     </row>
     <row r="131" spans="1:10">
       <c r="A131">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="B131">
         <v>34</v>
@@ -9995,7 +9995,7 @@
     </row>
     <row r="132" spans="1:10">
       <c r="A132">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="B132">
         <v>36</v>
@@ -10027,7 +10027,7 @@
     </row>
     <row r="133" spans="1:10">
       <c r="A133">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="B133">
         <v>24</v>
@@ -10059,7 +10059,7 @@
     </row>
     <row r="134" spans="1:10">
       <c r="A134">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="B134">
         <v>30</v>
@@ -10091,7 +10091,7 @@
     </row>
     <row r="135" spans="1:10">
       <c r="A135">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="B135">
         <v>23</v>
@@ -10123,7 +10123,7 @@
     </row>
     <row r="136" spans="1:10">
       <c r="A136">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="B136">
         <v>39</v>
@@ -10155,7 +10155,7 @@
     </row>
     <row r="137" spans="1:10">
       <c r="A137">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="B137">
         <v>37</v>
@@ -10187,7 +10187,7 @@
     </row>
     <row r="138" spans="1:10">
       <c r="A138">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="B138">
         <v>34</v>
@@ -10219,7 +10219,7 @@
     </row>
     <row r="139" spans="1:10">
       <c r="A139">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="B139">
         <v>36</v>
@@ -10251,7 +10251,7 @@
     </row>
     <row r="140" spans="1:10">
       <c r="A140">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="B140">
         <v>50</v>
@@ -10283,7 +10283,7 @@
     </row>
     <row r="141" spans="1:10">
       <c r="A141">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="B141">
         <v>22</v>
@@ -10315,7 +10315,7 @@
     </row>
     <row r="142" spans="1:10">
       <c r="A142">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="B142">
         <v>65</v>
@@ -10347,7 +10347,7 @@
     </row>
     <row r="143" spans="1:10">
       <c r="A143">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="B143">
         <v>26</v>
@@ -10379,7 +10379,7 @@
     </row>
     <row r="144" spans="1:10">
       <c r="A144">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="B144">
         <v>26</v>
@@ -10411,7 +10411,7 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="B145">
         <v>30</v>
@@ -10443,7 +10443,7 @@
     </row>
     <row r="146" spans="1:10">
       <c r="A146">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="B146">
         <v>28</v>
@@ -10475,7 +10475,7 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="B147">
         <v>57</v>
@@ -10507,7 +10507,7 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="B148">
         <v>62</v>
@@ -10539,7 +10539,7 @@
     </row>
     <row r="149" spans="1:10">
       <c r="A149">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="B149">
         <v>61</v>
@@ -10571,7 +10571,7 @@
     </row>
     <row r="150" spans="1:10">
       <c r="A150">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="B150">
         <v>43</v>
@@ -10603,7 +10603,7 @@
     </row>
     <row r="151" spans="1:10">
       <c r="A151">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="B151">
         <v>26</v>

</xml_diff>